<commit_message>
updated, trading high on buyout rumors from PSKY
</commit_message>
<xml_diff>
--- a/Media/WBD.xlsx
+++ b/Media/WBD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameel/Library/CloudStorage/Dropbox/models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameelbrannon/Library/CloudStorage/Dropbox/models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B9DD1D-1228-5A47-9D99-A587B5DD5D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5781EA2-9F67-7640-A33A-43D7B2B58953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="4220" windowWidth="34420" windowHeight="16940" activeTab="2" xr2:uid="{BDC8575E-1F7B-8A4D-8CF5-83B2922DCE33}"/>
+    <workbookView xWindow="7080" yWindow="4220" windowWidth="34420" windowHeight="16940" xr2:uid="{BDC8575E-1F7B-8A4D-8CF5-83B2922DCE33}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1456,7 +1456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5F5087-14B9-D049-974A-2BEFD66A4854}">
   <dimension ref="B2:S33"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="109" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="109" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -2141,8 +2141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B73814B-7DAF-874E-8EFC-8A7C9AA913FC}">
   <dimension ref="B2:HZ108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="O7" sqref="O7"/>
@@ -5664,27 +5664,27 @@
         <v>184</v>
       </c>
       <c r="C44" s="2">
-        <f>SUM(C36:C43)</f>
+        <f t="shared" ref="C44:H44" si="39">SUM(C36:C43)</f>
         <v>119819</v>
       </c>
       <c r="D44" s="2">
-        <f>SUM(D36:D43)</f>
+        <f t="shared" si="39"/>
         <v>108029</v>
       </c>
       <c r="E44" s="2">
-        <f>SUM(E36:E43)</f>
+        <f t="shared" si="39"/>
         <v>106333</v>
       </c>
       <c r="F44" s="2">
-        <f>SUM(F36:F43)</f>
+        <f t="shared" si="39"/>
         <v>104560</v>
       </c>
       <c r="G44" s="2">
-        <f>SUM(G36:G43)</f>
+        <f t="shared" si="39"/>
         <v>101679</v>
       </c>
       <c r="H44" s="2">
-        <f>SUM(H36:H43)</f>
+        <f t="shared" si="39"/>
         <v>101727</v>
       </c>
     </row>
@@ -5854,27 +5854,27 @@
         <v>192</v>
       </c>
       <c r="C53" s="2">
-        <f>+SUM(C46:C52)</f>
+        <f t="shared" ref="C53:H53" si="40">+SUM(C46:C52)</f>
         <v>74525</v>
       </c>
       <c r="D53" s="2">
-        <f>+SUM(D46:D52)</f>
+        <f t="shared" si="40"/>
         <v>72614</v>
       </c>
       <c r="E53" s="2">
-        <f>+SUM(E46:E52)</f>
+        <f t="shared" si="40"/>
         <v>70159</v>
       </c>
       <c r="F53" s="2">
-        <f>+SUM(F46:F52)</f>
+        <f t="shared" si="40"/>
         <v>69622</v>
       </c>
       <c r="G53" s="2">
-        <f>+SUM(G46:G52)</f>
+        <f t="shared" si="40"/>
         <v>66508</v>
       </c>
       <c r="H53" s="2">
-        <f>+SUM(H46:H52)</f>
+        <f t="shared" si="40"/>
         <v>64381</v>
       </c>
     </row>
@@ -5909,27 +5909,27 @@
         <v>194</v>
       </c>
       <c r="C55" s="2">
-        <f>+SUM(C53:C54)</f>
+        <f t="shared" ref="C55:H55" si="41">+SUM(C53:C54)</f>
         <v>119819</v>
       </c>
       <c r="D55" s="2">
-        <f>+SUM(D53:D54)</f>
+        <f t="shared" si="41"/>
         <v>108029</v>
       </c>
       <c r="E55" s="2">
-        <f>+SUM(E53:E54)</f>
+        <f t="shared" si="41"/>
         <v>106333</v>
       </c>
       <c r="F55" s="2">
-        <f>+SUM(F53:F54)</f>
+        <f t="shared" si="41"/>
         <v>104451</v>
       </c>
       <c r="G55" s="2">
-        <f>+SUM(G53:G54)</f>
+        <f t="shared" si="41"/>
         <v>101656</v>
       </c>
       <c r="H55" s="2">
-        <f>+SUM(H53:H54)</f>
+        <f t="shared" si="41"/>
         <v>101704</v>
       </c>
     </row>
@@ -5938,27 +5938,27 @@
         <v>195</v>
       </c>
       <c r="C57" s="2">
-        <f>SUM(C49:C50)</f>
+        <f t="shared" ref="C57:H57" si="42">SUM(C49:C50)</f>
         <v>42578</v>
       </c>
       <c r="D57" s="2">
-        <f>SUM(D49:D50)</f>
+        <f t="shared" si="42"/>
         <v>40958</v>
       </c>
       <c r="E57" s="2">
-        <f>SUM(E49:E50)</f>
+        <f t="shared" si="42"/>
         <v>40209</v>
       </c>
       <c r="F57" s="2">
-        <f>SUM(F49:F50)</f>
+        <f t="shared" si="42"/>
         <v>39505</v>
       </c>
       <c r="G57" s="2">
-        <f>SUM(G49:G50)</f>
+        <f t="shared" si="42"/>
         <v>37426</v>
       </c>
       <c r="H57" s="2">
-        <f>SUM(H49:H50)</f>
+        <f t="shared" si="42"/>
         <v>34632</v>
       </c>
     </row>
@@ -5967,27 +5967,27 @@
         <v>196</v>
       </c>
       <c r="C58" s="2">
-        <f>+C57+C54</f>
+        <f t="shared" ref="C58:H58" si="43">+C57+C54</f>
         <v>87872</v>
       </c>
       <c r="D58" s="2">
-        <f>+D57+D54</f>
+        <f t="shared" si="43"/>
         <v>76373</v>
       </c>
       <c r="E58" s="2">
-        <f>+E57+E54</f>
+        <f t="shared" si="43"/>
         <v>76383</v>
       </c>
       <c r="F58" s="2">
-        <f>+F57+F54</f>
+        <f t="shared" si="43"/>
         <v>74334</v>
       </c>
       <c r="G58" s="2">
-        <f>+G57+G54</f>
+        <f t="shared" si="43"/>
         <v>72574</v>
       </c>
       <c r="H58" s="2">
-        <f>+H57+H54</f>
+        <f t="shared" si="43"/>
         <v>71955</v>
       </c>
     </row>
@@ -5996,27 +5996,27 @@
         <v>197</v>
       </c>
       <c r="C59" s="7">
-        <f>+C57/C58</f>
+        <f t="shared" ref="C59:H59" si="44">+C57/C58</f>
         <v>0.48454570284049525</v>
       </c>
       <c r="D59" s="7">
-        <f>+D57/D58</f>
+        <f t="shared" si="44"/>
         <v>0.53628900265800739</v>
       </c>
       <c r="E59" s="7">
-        <f>+E57/E58</f>
+        <f t="shared" si="44"/>
         <v>0.52641294528887317</v>
       </c>
       <c r="F59" s="7">
-        <f>+F57/F58</f>
+        <f t="shared" si="44"/>
         <v>0.5314526327118142</v>
       </c>
       <c r="G59" s="7">
-        <f>+G57/G58</f>
+        <f t="shared" si="44"/>
         <v>0.51569432579160579</v>
       </c>
       <c r="H59" s="7">
-        <f>+H57/H58</f>
+        <f t="shared" si="44"/>
         <v>0.4813008130081301</v>
       </c>
     </row>
@@ -6029,23 +6029,23 @@
         <v>-39602</v>
       </c>
       <c r="D60" s="2">
-        <f t="shared" ref="D60:H60" si="39">+D36-D57</f>
+        <f t="shared" ref="D60:H60" si="45">+D36-D57</f>
         <v>-37345</v>
       </c>
       <c r="E60" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>-36873</v>
       </c>
       <c r="F60" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>-34193</v>
       </c>
       <c r="G60" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>-33558</v>
       </c>
       <c r="H60" s="2">
-        <f t="shared" si="39"/>
+        <f t="shared" si="45"/>
         <v>-29744</v>
       </c>
     </row>
@@ -6728,27 +6728,27 @@
         <v>39</v>
       </c>
       <c r="C104" s="2">
-        <f t="shared" ref="C104:H104" si="40">+SUM(C102:C103)</f>
+        <f t="shared" ref="C104:H104" si="46">+SUM(C102:C103)</f>
         <v>390</v>
       </c>
       <c r="D104" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>976</v>
       </c>
       <c r="E104" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>632</v>
       </c>
       <c r="F104" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>2429</v>
       </c>
       <c r="G104" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>302</v>
       </c>
       <c r="H104" s="2">
-        <f t="shared" si="40"/>
+        <f t="shared" si="46"/>
         <v>702</v>
       </c>
       <c r="U104" s="2">
@@ -6768,39 +6768,39 @@
         <v>4427</v>
       </c>
       <c r="Y104" s="2">
-        <f t="shared" ref="Y104:AG104" si="41">+X104*1</f>
+        <f t="shared" ref="Y104:AG104" si="47">+X104*1</f>
         <v>4427</v>
       </c>
       <c r="Z104" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>4427</v>
       </c>
       <c r="AA104" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>4427</v>
       </c>
       <c r="AB104" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>4427</v>
       </c>
       <c r="AC104" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>4427</v>
       </c>
       <c r="AD104" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>4427</v>
       </c>
       <c r="AE104" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>4427</v>
       </c>
       <c r="AF104" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>4427</v>
       </c>
       <c r="AG104" s="2">
-        <f t="shared" si="41"/>
+        <f t="shared" si="47"/>
         <v>4427</v>
       </c>
       <c r="AH104" s="2">

</xml_diff>